<commit_message>
identifiquei o caso do perfslope
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/tabelas_analise_formatada.xlsx
+++ b/models/dissertation-model/modelo-R/tabelas_analise_formatada.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ParametrosCalibracao" sheetId="1" r:id="rId1"/>
@@ -23,17 +23,19 @@
     <sheet name="RankingVariaveisRandomForest" sheetId="8" r:id="rId9"/>
     <sheet name="RankingVariaveisBoruta" sheetId="9" r:id="rId10"/>
     <sheet name="RankingGeral" sheetId="10" r:id="rId11"/>
+    <sheet name="RankingGeral_Modo2" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">DataFraneVulnerabilidade!$A$1:$AM$201</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">EstratégiasTestadas!$A$1:$D$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">RankingGeral_Modo2!$A$1:$L$36</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="240">
   <si>
     <t>Variavel</t>
   </si>
@@ -736,6 +738,24 @@
   <si>
     <t>Teste t</t>
   </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
 </sst>
 </file>
 
@@ -747,7 +767,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -814,6 +834,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -865,7 +893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1014,7 +1042,25 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1029,23 +1075,13 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5536,7 +5572,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6159,6 +6195,1542 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00B187AC-06E3-439A-B7D8-1EBFAABEB01E}">
+  <dimension ref="A1:L36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="6.5703125" style="32" customWidth="1"/>
+    <col min="8" max="11" width="30.28515625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" style="29" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>237</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="68" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>230</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="J1" s="39" t="s">
+        <v>232</v>
+      </c>
+      <c r="K1" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="L1" s="38" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="32">
+        <f>VLOOKUP(A2,$H:$L,5,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="32">
+        <f>VLOOKUP(A2,$I:$L,4,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="32">
+        <f>VLOOKUP(A2,$J:$L,3,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="E2" s="32">
+        <f>VLOOKUP(A2,$K:$L,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="F2" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="G2" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="I2" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="J2" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="32">
+        <f>VLOOKUP(A3,$H:$L,5,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="32">
+        <f>VLOOKUP(A3,$I:$L,4,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D3" s="32">
+        <f>VLOOKUP(A3,$J:$L,3,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="32">
+        <f>VLOOKUP(A3,$K:$L,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="G3" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="K3" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="L3" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="32">
+        <f>VLOOKUP(A4,$H:$L,5,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="C4" s="32">
+        <f>VLOOKUP(A4,$I:$L,4,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="32">
+        <f>VLOOKUP(A4,$J:$L,3,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="E4" s="32">
+        <f>VLOOKUP(A4,$K:$L,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="F4" s="32">
+        <v>4</v>
+      </c>
+      <c r="G4" s="32">
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="I4" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="L4" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="32">
+        <f>VLOOKUP(A5,$H:$L,5,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="C5" s="32">
+        <f>VLOOKUP(A5,$I:$L,4,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="D5" s="32">
+        <f>VLOOKUP(A5,$J:$L,3,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="E5" s="32">
+        <f>VLOOKUP(A5,$K:$L,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="F5" s="32">
+        <v>6</v>
+      </c>
+      <c r="G5" s="32">
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="H5" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="K5" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="32">
+        <f>VLOOKUP(A6,$H:$L,5,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="C6" s="32">
+        <f>VLOOKUP(A6,$I:$L,4,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="D6" s="32">
+        <f>VLOOKUP(A6,$J:$L,3,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="E6" s="32">
+        <f>VLOOKUP(A6,$K:$L,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="F6" s="32">
+        <v>8.75</v>
+      </c>
+      <c r="G6" s="32">
+        <v>0.82915619758884995</v>
+      </c>
+      <c r="H6" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="K6" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="L6" s="29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="32">
+        <f>VLOOKUP(A7,$H:$L,5,FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="C7" s="32">
+        <f>VLOOKUP(A7,$I:$L,4,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="D7" s="32">
+        <f>VLOOKUP(A7,$J:$L,3,FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="E7" s="32">
+        <f>VLOOKUP(A7,$K:$L,2,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="F7" s="32">
+        <v>28.25</v>
+      </c>
+      <c r="G7" s="32">
+        <v>1.0897247358851685</v>
+      </c>
+      <c r="H7" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="L7" s="29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="32">
+        <f>VLOOKUP(A8,$H:$L,5,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="C8" s="32">
+        <f>VLOOKUP(A8,$I:$L,4,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="D8" s="32">
+        <f>VLOOKUP(A8,$J:$L,3,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="E8" s="32">
+        <f>VLOOKUP(A8,$K:$L,2,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="F8" s="32">
+        <v>12.5</v>
+      </c>
+      <c r="G8" s="32">
+        <v>1.1180339887498949</v>
+      </c>
+      <c r="H8" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="J8" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="L8" s="29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="32">
+        <f>VLOOKUP(A9,$H:$L,5,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="C9" s="32">
+        <f>VLOOKUP(A9,$I:$L,4,FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="D9" s="32">
+        <f>VLOOKUP(A9,$J:$L,3,FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="E9" s="32">
+        <f>VLOOKUP(A9,$K:$L,2,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="F9" s="32">
+        <v>30.25</v>
+      </c>
+      <c r="G9" s="32">
+        <v>1.479019945774904</v>
+      </c>
+      <c r="H9" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="L9" s="29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="32">
+        <f>VLOOKUP(A10,$H:$L,5,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="C10" s="32">
+        <f>VLOOKUP(A10,$I:$L,4,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="D10" s="32">
+        <f>VLOOKUP(A10,$J:$L,3,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="E10" s="32">
+        <f>VLOOKUP(A10,$K:$L,2,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="F10" s="32">
+        <v>15.75</v>
+      </c>
+      <c r="G10" s="32">
+        <v>1.6393596310755001</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="L10" s="29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="32">
+        <f>VLOOKUP(A11,$H:$L,5,FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="C11" s="32">
+        <f>VLOOKUP(A11,$I:$L,4,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="D11" s="32">
+        <f>VLOOKUP(A11,$J:$L,3,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="E11" s="32">
+        <f>VLOOKUP(A11,$K:$L,2,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="F11" s="32">
+        <v>18.75</v>
+      </c>
+      <c r="G11" s="32">
+        <v>1.6393596310755001</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="K11" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="L11" s="29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="32">
+        <f>VLOOKUP(A12,$H:$L,5,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="C12" s="32">
+        <f>VLOOKUP(A12,$I:$L,4,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D12" s="32">
+        <f>VLOOKUP(A12,$J:$L,3,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="E12" s="32">
+        <f>VLOOKUP(A12,$K:$L,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="F12" s="32">
+        <v>5.25</v>
+      </c>
+      <c r="G12" s="32">
+        <v>1.7853571071357126</v>
+      </c>
+      <c r="H12" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="J12" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="32">
+        <f>VLOOKUP(A13,$H:$L,5,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="C13" s="32">
+        <f>VLOOKUP(A13,$I:$L,4,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="D13" s="32">
+        <f>VLOOKUP(A13,$J:$L,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="E13" s="32">
+        <f>VLOOKUP(A13,$K:$L,2,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="F13" s="32">
+        <v>14.5</v>
+      </c>
+      <c r="G13" s="32">
+        <v>2.0615528128088303</v>
+      </c>
+      <c r="H13" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="I13" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="K13" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="L13" s="29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="32">
+        <f>VLOOKUP(A14,$H:$L,5,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="C14" s="32">
+        <f>VLOOKUP(A14,$I:$L,4,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="D14" s="32">
+        <f>VLOOKUP(A14,$J:$L,3,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="E14" s="32">
+        <f>VLOOKUP(A14,$K:$L,2,FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="F14" s="32">
+        <v>19.5</v>
+      </c>
+      <c r="G14" s="32">
+        <v>2.0615528128088303</v>
+      </c>
+      <c r="H14" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="I14" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="J14" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="K14" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="L14" s="29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="32">
+        <f>VLOOKUP(A15,$H:$L,5,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="C15" s="32">
+        <f>VLOOKUP(A15,$I:$L,4,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="D15" s="32">
+        <f>VLOOKUP(A15,$J:$L,3,FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="E15" s="32">
+        <f>VLOOKUP(A15,$K:$L,2,FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="F15" s="32">
+        <v>20.5</v>
+      </c>
+      <c r="G15" s="32">
+        <v>2.0615528128088303</v>
+      </c>
+      <c r="H15" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="J15" s="54" t="s">
+        <v>152</v>
+      </c>
+      <c r="K15" s="54" t="s">
+        <v>152</v>
+      </c>
+      <c r="L15" s="29">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="32">
+        <f>VLOOKUP(A16,$H:$L,5,FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="C16" s="32">
+        <f>VLOOKUP(A16,$I:$L,4,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="D16" s="32">
+        <f>VLOOKUP(A16,$J:$L,3,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="E16" s="32">
+        <f>VLOOKUP(A16,$K:$L,2,FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="F16" s="32">
+        <v>30.75</v>
+      </c>
+      <c r="G16" s="32">
+        <v>2.2776083947860748</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="I16" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="J16" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="K16" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="L16" s="29">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" s="32">
+        <f>VLOOKUP(A17,$H:$L,5,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="C17" s="32">
+        <f>VLOOKUP(A17,$I:$L,4,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="D17" s="32">
+        <f>VLOOKUP(A17,$J:$L,3,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="E17" s="32">
+        <f>VLOOKUP(A17,$K:$L,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="F17" s="32">
+        <v>7.5</v>
+      </c>
+      <c r="G17" s="32">
+        <v>2.2912878474779199</v>
+      </c>
+      <c r="H17" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="I17" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="J17" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="K17" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="L17" s="29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="69" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="32">
+        <f>VLOOKUP(A18,$H:$L,5,FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="C18" s="32">
+        <f>VLOOKUP(A18,$I:$L,4,FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="D18" s="32">
+        <f>VLOOKUP(A18,$J:$L,3,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="E18" s="32">
+        <f>VLOOKUP(A18,$K:$L,2,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="F18" s="32">
+        <v>32.5</v>
+      </c>
+      <c r="G18" s="32">
+        <v>2.5</v>
+      </c>
+      <c r="H18" s="69" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="69" t="s">
+        <v>118</v>
+      </c>
+      <c r="J18" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="K18" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="L18" s="70">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="32">
+        <f>VLOOKUP(A19,$H:$L,5,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="C19" s="32">
+        <f>VLOOKUP(A19,$I:$L,4,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="D19" s="32">
+        <f>VLOOKUP(A19,$J:$L,3,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="E19" s="32">
+        <f>VLOOKUP(A19,$K:$L,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="F19" s="32">
+        <v>5.5</v>
+      </c>
+      <c r="G19" s="32">
+        <v>2.598076211353316</v>
+      </c>
+      <c r="H19" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="32">
+        <f>VLOOKUP(A20,$H:$L,5,FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="C20" s="32">
+        <f>VLOOKUP(A20,$I:$L,4,FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="D20" s="32">
+        <f>VLOOKUP(A20,$J:$L,3,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="E20" s="32">
+        <f>VLOOKUP(A20,$K:$L,2,FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="F20" s="32">
+        <v>27.75</v>
+      </c>
+      <c r="G20" s="32">
+        <v>3.1124748994971831</v>
+      </c>
+      <c r="H20" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="I20" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="K20" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="32">
+        <f>VLOOKUP(A21,$H:$L,5,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="C21" s="32">
+        <f>VLOOKUP(A21,$I:$L,4,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="D21" s="32">
+        <f>VLOOKUP(A21,$J:$L,3,FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="E21" s="32">
+        <f>VLOOKUP(A21,$K:$L,2,FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="F21" s="32">
+        <v>28.25</v>
+      </c>
+      <c r="G21" s="32">
+        <v>3.7666297933298409</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="J21" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="K21" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="L21" s="29">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="32">
+        <f>VLOOKUP(A22,$H:$L,5,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="C22" s="32">
+        <f>VLOOKUP(A22,$I:$L,4,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="D22" s="32">
+        <f>VLOOKUP(A22,$J:$L,3,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="E22" s="32">
+        <f>VLOOKUP(A22,$K:$L,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="F22" s="32">
+        <v>10.75</v>
+      </c>
+      <c r="G22" s="32">
+        <v>3.8324274291889728</v>
+      </c>
+      <c r="H22" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="J22" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="K22" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="L22" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="32">
+        <f>VLOOKUP(A23,$H:$L,5,FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="C23" s="32">
+        <f>VLOOKUP(A23,$I:$L,4,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="D23" s="32">
+        <f>VLOOKUP(A23,$J:$L,3,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="E23" s="32">
+        <f>VLOOKUP(A23,$K:$L,2,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="F23" s="32">
+        <v>23.25</v>
+      </c>
+      <c r="G23" s="32">
+        <v>3.897114317029974</v>
+      </c>
+      <c r="H23" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="J23" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="K23" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="L23" s="29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="32">
+        <f>VLOOKUP(A24,$H:$L,5,FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="C24" s="32">
+        <f>VLOOKUP(A24,$I:$L,4,FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="D24" s="32">
+        <f>VLOOKUP(A24,$J:$L,3,FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="E24" s="32">
+        <f>VLOOKUP(A24,$K:$L,2,FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="F24" s="32">
+        <v>25.75</v>
+      </c>
+      <c r="G24" s="32">
+        <v>4.0850336595920478</v>
+      </c>
+      <c r="H24" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="I24" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="J24" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="K24" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="L24" s="29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="54" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="32">
+        <f>VLOOKUP(A25,$H:$L,5,FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="C25" s="32">
+        <f>VLOOKUP(A25,$I:$L,4,FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="D25" s="32">
+        <f>VLOOKUP(A25,$J:$L,3,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="E25" s="32">
+        <f>VLOOKUP(A25,$K:$L,2,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="F25" s="32">
+        <v>24.25</v>
+      </c>
+      <c r="G25" s="32">
+        <v>4.0850336595920478</v>
+      </c>
+      <c r="H25" s="54" t="s">
+        <v>152</v>
+      </c>
+      <c r="I25" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="K25" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="L25" s="29">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="32">
+        <f>VLOOKUP(A26,$H:$L,5,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="C26" s="32">
+        <f>VLOOKUP(A26,$I:$L,4,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D26" s="32">
+        <f>VLOOKUP(A26,$J:$L,3,FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="E26" s="32">
+        <f>VLOOKUP(A26,$K:$L,2,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="F26" s="32">
+        <v>19.75</v>
+      </c>
+      <c r="G26" s="32">
+        <v>4.4370598373247123</v>
+      </c>
+      <c r="H26" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="I26" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="J26" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="K26" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="L26" s="29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="32">
+        <f>VLOOKUP(A27,$H:$L,5,FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="C27" s="32">
+        <f>VLOOKUP(A27,$I:$L,4,FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="D27" s="32">
+        <f>VLOOKUP(A27,$J:$L,3,FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="E27" s="32">
+        <f>VLOOKUP(A27,$K:$L,2,FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="F27" s="32">
+        <v>29</v>
+      </c>
+      <c r="G27" s="32">
+        <v>4.5276925690687087</v>
+      </c>
+      <c r="H27" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="I27" s="54" t="s">
+        <v>152</v>
+      </c>
+      <c r="J27" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="K27" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="L27" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="32">
+        <f>VLOOKUP(A28,$H:$L,5,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="C28" s="32">
+        <f>VLOOKUP(A28,$I:$L,4,FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="D28" s="32">
+        <f>VLOOKUP(A28,$J:$L,3,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="E28" s="32">
+        <f>VLOOKUP(A28,$K:$L,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="F28" s="32">
+        <v>13.75</v>
+      </c>
+      <c r="G28" s="32">
+        <v>4.815340071064556</v>
+      </c>
+      <c r="H28" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="I28" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="J28" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="K28" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="L28" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" s="32">
+        <f>VLOOKUP(A29,$H:$L,5,FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="C29" s="32">
+        <f>VLOOKUP(A29,$I:$L,4,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="D29" s="32">
+        <f>VLOOKUP(A29,$J:$L,3,FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="E29" s="32">
+        <f>VLOOKUP(A29,$K:$L,2,FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="F29" s="32">
+        <v>30.5</v>
+      </c>
+      <c r="G29" s="32">
+        <v>5.5</v>
+      </c>
+      <c r="H29" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="I29" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="J29" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="K29" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="L29" s="29">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="32">
+        <f>VLOOKUP(A30,$H:$L,5,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="C30" s="32">
+        <f>VLOOKUP(A30,$I:$L,4,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="D30" s="32">
+        <f>VLOOKUP(A30,$J:$L,3,FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="E30" s="32">
+        <f>VLOOKUP(A30,$K:$L,2,FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="F30" s="32">
+        <v>20</v>
+      </c>
+      <c r="G30" s="32">
+        <v>5.5226805085936306</v>
+      </c>
+      <c r="H30" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="I30" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="J30" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="K30" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="L30" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="B31" s="32">
+        <f>VLOOKUP(A31,$H:$L,5,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="C31" s="32">
+        <f>VLOOKUP(A31,$I:$L,4,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="D31" s="32">
+        <f>VLOOKUP(A31,$J:$L,3,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="E31" s="32">
+        <f>VLOOKUP(A31,$K:$L,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="F31" s="32">
+        <v>15.75</v>
+      </c>
+      <c r="G31" s="32">
+        <v>5.8470077817632502</v>
+      </c>
+      <c r="H31" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="I31" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="J31" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="K31" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="L31" s="29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" s="32">
+        <f>VLOOKUP(A32,$H:$L,5,FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="C32" s="32">
+        <f>VLOOKUP(A32,$I:$L,4,FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="D32" s="32">
+        <f>VLOOKUP(A32,$J:$L,3,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="E32" s="32">
+        <f>VLOOKUP(A32,$K:$L,2,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="F32" s="32">
+        <v>18.25</v>
+      </c>
+      <c r="G32" s="32">
+        <v>5.9319052588523364</v>
+      </c>
+      <c r="H32" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="I32" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="J32" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="K32" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="L32" s="29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="32">
+        <f>VLOOKUP(A33,$H:$L,5,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="C33" s="32">
+        <f>VLOOKUP(A33,$I:$L,4,FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="D33" s="32">
+        <f>VLOOKUP(A33,$J:$L,3,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="E33" s="32">
+        <f>VLOOKUP(A33,$K:$L,2,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="F33" s="32">
+        <v>19</v>
+      </c>
+      <c r="G33" s="32">
+        <v>6.9641941385920596</v>
+      </c>
+      <c r="H33" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="J33" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="K33" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="L33" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" s="32">
+        <f>VLOOKUP(A34,$H:$L,5,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="C34" s="32">
+        <f>VLOOKUP(A34,$I:$L,4,FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="D34" s="32">
+        <f>VLOOKUP(A34,$J:$L,3,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="E34" s="32">
+        <f>VLOOKUP(A34,$K:$L,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="F34" s="32">
+        <v>15.25</v>
+      </c>
+      <c r="G34" s="32">
+        <v>8.1967981553775004</v>
+      </c>
+      <c r="H34" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="I34" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="J34" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="K34" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="L34" s="29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="32">
+        <f>VLOOKUP(A35,$H:$L,5,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="C35" s="32">
+        <f>VLOOKUP(A35,$I:$L,4,FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="D35" s="32">
+        <f>VLOOKUP(A35,$J:$L,3,FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="E35" s="32">
+        <f>VLOOKUP(A35,$K:$L,2,FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="F35" s="32">
+        <v>29.75</v>
+      </c>
+      <c r="G35" s="32">
+        <v>8.5256964524899672</v>
+      </c>
+      <c r="H35" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="I35" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="J35" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="K35" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="L35" s="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="32">
+        <f>VLOOKUP(A36,$H:$L,5,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="C36" s="32">
+        <f>VLOOKUP(A36,$I:$L,4,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="D36" s="32">
+        <f>VLOOKUP(A36,$J:$L,3,FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="E36" s="32">
+        <f>VLOOKUP(A36,$K:$L,2,FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="F36" s="32">
+        <v>15.75</v>
+      </c>
+      <c r="G36" s="32">
+        <v>11.277743568639961</v>
+      </c>
+      <c r="H36" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="I36" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="J36" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="K36" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="L36" s="30">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:L36" xr:uid="{A962AB0A-45DE-4224-AD9F-13578AB1821C}">
+    <sortState ref="A2:L36">
+      <sortCondition ref="G1:G36"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -7093,15 +8665,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="60" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="62" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7121,920 +8693,920 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62">
+      <c r="A3" s="56">
         <v>1</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C3" s="63">
+      <c r="C3" s="57">
         <v>0.3</v>
       </c>
-      <c r="D3" s="63">
+      <c r="D3" s="57">
         <v>0.1</v>
       </c>
-      <c r="E3" s="63">
+      <c r="E3" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62">
+      <c r="A4" s="56">
         <v>2</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C4" s="63">
+      <c r="C4" s="57">
         <v>0.3</v>
       </c>
-      <c r="D4" s="63">
+      <c r="D4" s="57">
         <v>0.1</v>
       </c>
-      <c r="E4" s="63">
+      <c r="E4" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62">
+      <c r="A5" s="56">
         <v>3</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C5" s="63">
+      <c r="C5" s="57">
         <v>0.3</v>
       </c>
-      <c r="D5" s="63">
+      <c r="D5" s="57">
         <v>0.1</v>
       </c>
-      <c r="E5" s="63">
+      <c r="E5" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62">
+      <c r="A6" s="56">
         <v>4</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="63">
+      <c r="C6" s="57">
         <v>0.3</v>
       </c>
-      <c r="D6" s="63">
+      <c r="D6" s="57">
         <v>0.1</v>
       </c>
-      <c r="E6" s="63">
+      <c r="E6" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62">
+      <c r="A7" s="56">
         <v>5</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C7" s="63">
+      <c r="C7" s="57">
         <v>0.3</v>
       </c>
-      <c r="D7" s="63">
+      <c r="D7" s="57">
         <v>0.1</v>
       </c>
-      <c r="E7" s="63">
+      <c r="E7" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="62">
+      <c r="A8" s="56">
         <v>6</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C8" s="63">
+      <c r="C8" s="57">
         <v>0.3</v>
       </c>
-      <c r="D8" s="63">
+      <c r="D8" s="57">
         <v>0.1</v>
       </c>
-      <c r="E8" s="63">
+      <c r="E8" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="62">
+      <c r="A9" s="56">
         <v>7</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C9" s="63">
+      <c r="C9" s="57">
         <v>0.2</v>
       </c>
-      <c r="D9" s="63">
+      <c r="D9" s="57">
         <v>0.1</v>
       </c>
-      <c r="E9" s="63">
+      <c r="E9" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62">
+      <c r="A10" s="56">
         <v>8</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C10" s="63">
+      <c r="C10" s="57">
         <v>0.2</v>
       </c>
-      <c r="D10" s="63">
+      <c r="D10" s="57">
         <v>0.1</v>
       </c>
-      <c r="E10" s="63">
+      <c r="E10" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="62">
+      <c r="A11" s="56">
         <v>9</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C11" s="63">
+      <c r="C11" s="57">
         <v>0.2</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="57">
         <v>0.1</v>
       </c>
-      <c r="E11" s="63">
+      <c r="E11" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="62">
+      <c r="A12" s="56">
         <v>10</v>
       </c>
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C12" s="63">
+      <c r="C12" s="57">
         <v>0.2</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="57">
         <v>0.1</v>
       </c>
-      <c r="E12" s="63">
+      <c r="E12" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="62">
+      <c r="A13" s="56">
         <v>11</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="63">
+      <c r="C13" s="57">
         <v>0.2</v>
       </c>
-      <c r="D13" s="63">
+      <c r="D13" s="57">
         <v>0.1</v>
       </c>
-      <c r="E13" s="63">
+      <c r="E13" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="62">
+      <c r="A14" s="56">
         <v>12</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="63">
+      <c r="C14" s="57">
         <v>0.2</v>
       </c>
-      <c r="D14" s="63">
+      <c r="D14" s="57">
         <v>0.1</v>
       </c>
-      <c r="E14" s="63">
+      <c r="E14" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="62">
+      <c r="A15" s="56">
         <v>13</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C15" s="63">
+      <c r="C15" s="57">
         <v>0.4</v>
       </c>
-      <c r="D15" s="63">
+      <c r="D15" s="57">
         <v>0.1</v>
       </c>
-      <c r="E15" s="63">
+      <c r="E15" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="62">
+      <c r="A16" s="56">
         <v>14</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C16" s="63">
+      <c r="C16" s="57">
         <v>0.4</v>
       </c>
-      <c r="D16" s="63">
+      <c r="D16" s="57">
         <v>0.1</v>
       </c>
-      <c r="E16" s="63">
+      <c r="E16" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62">
+      <c r="A17" s="56">
         <v>15</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C17" s="63">
+      <c r="C17" s="57">
         <v>0.4</v>
       </c>
-      <c r="D17" s="63">
+      <c r="D17" s="57">
         <v>0.1</v>
       </c>
-      <c r="E17" s="63">
+      <c r="E17" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="62">
+      <c r="A18" s="56">
         <v>16</v>
       </c>
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C18" s="63">
+      <c r="C18" s="57">
         <v>0.4</v>
       </c>
-      <c r="D18" s="63">
+      <c r="D18" s="57">
         <v>0.1</v>
       </c>
-      <c r="E18" s="63">
+      <c r="E18" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="62">
+      <c r="A19" s="56">
         <v>17</v>
       </c>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C19" s="63">
+      <c r="C19" s="57">
         <v>0.4</v>
       </c>
-      <c r="D19" s="63">
+      <c r="D19" s="57">
         <v>0.1</v>
       </c>
-      <c r="E19" s="63">
+      <c r="E19" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="62">
+      <c r="A20" s="56">
         <v>18</v>
       </c>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="63">
+      <c r="C20" s="57">
         <v>0.4</v>
       </c>
-      <c r="D20" s="63">
+      <c r="D20" s="57">
         <v>0.1</v>
       </c>
-      <c r="E20" s="63">
+      <c r="E20" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="62">
+      <c r="A21" s="56">
         <v>19</v>
       </c>
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C21" s="63">
+      <c r="C21" s="57">
         <v>0.3</v>
       </c>
-      <c r="D21" s="63">
+      <c r="D21" s="57">
         <v>0.05</v>
       </c>
-      <c r="E21" s="63">
+      <c r="E21" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="62">
+      <c r="A22" s="56">
         <v>20</v>
       </c>
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C22" s="63">
+      <c r="C22" s="57">
         <v>0.3</v>
       </c>
-      <c r="D22" s="63">
+      <c r="D22" s="57">
         <v>0.05</v>
       </c>
-      <c r="E22" s="63">
+      <c r="E22" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="62">
+      <c r="A23" s="56">
         <v>21</v>
       </c>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C23" s="63">
+      <c r="C23" s="57">
         <v>0.3</v>
       </c>
-      <c r="D23" s="63">
+      <c r="D23" s="57">
         <v>0.05</v>
       </c>
-      <c r="E23" s="63">
+      <c r="E23" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="62">
+      <c r="A24" s="56">
         <v>22</v>
       </c>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C24" s="63">
+      <c r="C24" s="57">
         <v>0.3</v>
       </c>
-      <c r="D24" s="63">
+      <c r="D24" s="57">
         <v>0.05</v>
       </c>
-      <c r="E24" s="63">
+      <c r="E24" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="62">
+      <c r="A25" s="56">
         <v>23</v>
       </c>
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C25" s="63">
+      <c r="C25" s="57">
         <v>0.3</v>
       </c>
-      <c r="D25" s="63">
+      <c r="D25" s="57">
         <v>0.05</v>
       </c>
-      <c r="E25" s="63">
+      <c r="E25" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="62">
+      <c r="A26" s="56">
         <v>24</v>
       </c>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C26" s="63">
+      <c r="C26" s="57">
         <v>0.3</v>
       </c>
-      <c r="D26" s="63">
+      <c r="D26" s="57">
         <v>0.05</v>
       </c>
-      <c r="E26" s="63">
+      <c r="E26" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="62">
+      <c r="A27" s="56">
         <v>25</v>
       </c>
-      <c r="B27" s="62" t="s">
+      <c r="B27" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C27" s="63">
+      <c r="C27" s="57">
         <v>0.2</v>
       </c>
-      <c r="D27" s="63">
+      <c r="D27" s="57">
         <v>0.05</v>
       </c>
-      <c r="E27" s="63">
+      <c r="E27" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="62">
+      <c r="A28" s="56">
         <v>26</v>
       </c>
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C28" s="63">
+      <c r="C28" s="57">
         <v>0.2</v>
       </c>
-      <c r="D28" s="63">
+      <c r="D28" s="57">
         <v>0.05</v>
       </c>
-      <c r="E28" s="63">
+      <c r="E28" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="62">
+      <c r="A29" s="56">
         <v>27</v>
       </c>
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C29" s="63">
+      <c r="C29" s="57">
         <v>0.2</v>
       </c>
-      <c r="D29" s="63">
+      <c r="D29" s="57">
         <v>0.05</v>
       </c>
-      <c r="E29" s="63">
+      <c r="E29" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="62">
+      <c r="A30" s="56">
         <v>28</v>
       </c>
-      <c r="B30" s="62" t="s">
+      <c r="B30" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C30" s="63">
+      <c r="C30" s="57">
         <v>0.2</v>
       </c>
-      <c r="D30" s="63">
+      <c r="D30" s="57">
         <v>0.05</v>
       </c>
-      <c r="E30" s="63">
+      <c r="E30" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="62">
+      <c r="A31" s="56">
         <v>29</v>
       </c>
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C31" s="63">
+      <c r="C31" s="57">
         <v>0.2</v>
       </c>
-      <c r="D31" s="63">
+      <c r="D31" s="57">
         <v>0.05</v>
       </c>
-      <c r="E31" s="63">
+      <c r="E31" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="62">
+      <c r="A32" s="56">
         <v>30</v>
       </c>
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C32" s="63">
+      <c r="C32" s="57">
         <v>0.2</v>
       </c>
-      <c r="D32" s="63">
+      <c r="D32" s="57">
         <v>0.05</v>
       </c>
-      <c r="E32" s="63">
+      <c r="E32" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="62">
+      <c r="A33" s="56">
         <v>31</v>
       </c>
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C33" s="63">
+      <c r="C33" s="57">
         <v>0.4</v>
       </c>
-      <c r="D33" s="63">
+      <c r="D33" s="57">
         <v>0.05</v>
       </c>
-      <c r="E33" s="63">
+      <c r="E33" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="62">
+      <c r="A34" s="56">
         <v>32</v>
       </c>
-      <c r="B34" s="62" t="s">
+      <c r="B34" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C34" s="63">
+      <c r="C34" s="57">
         <v>0.4</v>
       </c>
-      <c r="D34" s="63">
+      <c r="D34" s="57">
         <v>0.05</v>
       </c>
-      <c r="E34" s="63">
+      <c r="E34" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="62">
+      <c r="A35" s="56">
         <v>33</v>
       </c>
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C35" s="63">
+      <c r="C35" s="57">
         <v>0.4</v>
       </c>
-      <c r="D35" s="63">
+      <c r="D35" s="57">
         <v>0.05</v>
       </c>
-      <c r="E35" s="63">
+      <c r="E35" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="62">
+      <c r="A36" s="56">
         <v>34</v>
       </c>
-      <c r="B36" s="62" t="s">
+      <c r="B36" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C36" s="63">
+      <c r="C36" s="57">
         <v>0.4</v>
       </c>
-      <c r="D36" s="63">
+      <c r="D36" s="57">
         <v>0.05</v>
       </c>
-      <c r="E36" s="63">
+      <c r="E36" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="62">
+      <c r="A37" s="56">
         <v>35</v>
       </c>
-      <c r="B37" s="62" t="s">
+      <c r="B37" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C37" s="63">
+      <c r="C37" s="57">
         <v>0.4</v>
       </c>
-      <c r="D37" s="63">
+      <c r="D37" s="57">
         <v>0.05</v>
       </c>
-      <c r="E37" s="63">
+      <c r="E37" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="62">
+      <c r="A38" s="56">
         <v>36</v>
       </c>
-      <c r="B38" s="62" t="s">
+      <c r="B38" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C38" s="63">
+      <c r="C38" s="57">
         <v>0.4</v>
       </c>
-      <c r="D38" s="63">
+      <c r="D38" s="57">
         <v>0.05</v>
       </c>
-      <c r="E38" s="63">
+      <c r="E38" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="62">
+      <c r="A39" s="56">
         <v>37</v>
       </c>
-      <c r="B39" s="62" t="s">
+      <c r="B39" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C39" s="63">
+      <c r="C39" s="57">
         <v>0.3</v>
       </c>
-      <c r="D39" s="63">
+      <c r="D39" s="57">
         <v>0.15</v>
       </c>
-      <c r="E39" s="63">
+      <c r="E39" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="62">
+      <c r="A40" s="56">
         <v>38</v>
       </c>
-      <c r="B40" s="62" t="s">
+      <c r="B40" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C40" s="63">
+      <c r="C40" s="57">
         <v>0.3</v>
       </c>
-      <c r="D40" s="63">
+      <c r="D40" s="57">
         <v>0.15</v>
       </c>
-      <c r="E40" s="63">
+      <c r="E40" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="62">
+      <c r="A41" s="56">
         <v>39</v>
       </c>
-      <c r="B41" s="62" t="s">
+      <c r="B41" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C41" s="63">
+      <c r="C41" s="57">
         <v>0.3</v>
       </c>
-      <c r="D41" s="63">
+      <c r="D41" s="57">
         <v>0.15</v>
       </c>
-      <c r="E41" s="63">
+      <c r="E41" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="62">
+      <c r="A42" s="56">
         <v>40</v>
       </c>
-      <c r="B42" s="62" t="s">
+      <c r="B42" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C42" s="63">
+      <c r="C42" s="57">
         <v>0.3</v>
       </c>
-      <c r="D42" s="63">
+      <c r="D42" s="57">
         <v>0.15</v>
       </c>
-      <c r="E42" s="63">
+      <c r="E42" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="62">
+      <c r="A43" s="56">
         <v>41</v>
       </c>
-      <c r="B43" s="62" t="s">
+      <c r="B43" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C43" s="63">
+      <c r="C43" s="57">
         <v>0.3</v>
       </c>
-      <c r="D43" s="63">
+      <c r="D43" s="57">
         <v>0.15</v>
       </c>
-      <c r="E43" s="63">
+      <c r="E43" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="62">
+      <c r="A44" s="56">
         <v>42</v>
       </c>
-      <c r="B44" s="62" t="s">
+      <c r="B44" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C44" s="63">
+      <c r="C44" s="57">
         <v>0.3</v>
       </c>
-      <c r="D44" s="63">
+      <c r="D44" s="57">
         <v>0.15</v>
       </c>
-      <c r="E44" s="63">
+      <c r="E44" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="62">
+      <c r="A45" s="56">
         <v>43</v>
       </c>
-      <c r="B45" s="62" t="s">
+      <c r="B45" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C45" s="63">
+      <c r="C45" s="57">
         <v>0.2</v>
       </c>
-      <c r="D45" s="63">
+      <c r="D45" s="57">
         <v>0.15</v>
       </c>
-      <c r="E45" s="63">
+      <c r="E45" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="62">
+      <c r="A46" s="56">
         <v>44</v>
       </c>
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C46" s="63">
+      <c r="C46" s="57">
         <v>0.2</v>
       </c>
-      <c r="D46" s="63">
+      <c r="D46" s="57">
         <v>0.15</v>
       </c>
-      <c r="E46" s="63">
+      <c r="E46" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="62">
+      <c r="A47" s="56">
         <v>45</v>
       </c>
-      <c r="B47" s="62" t="s">
+      <c r="B47" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="63">
+      <c r="C47" s="57">
         <v>0.2</v>
       </c>
-      <c r="D47" s="63">
+      <c r="D47" s="57">
         <v>0.15</v>
       </c>
-      <c r="E47" s="63">
+      <c r="E47" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="62">
+      <c r="A48" s="56">
         <v>46</v>
       </c>
-      <c r="B48" s="62" t="s">
+      <c r="B48" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C48" s="63">
+      <c r="C48" s="57">
         <v>0.2</v>
       </c>
-      <c r="D48" s="63">
+      <c r="D48" s="57">
         <v>0.15</v>
       </c>
-      <c r="E48" s="63">
+      <c r="E48" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="62">
+      <c r="A49" s="56">
         <v>47</v>
       </c>
-      <c r="B49" s="62" t="s">
+      <c r="B49" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C49" s="63">
+      <c r="C49" s="57">
         <v>0.2</v>
       </c>
-      <c r="D49" s="63">
+      <c r="D49" s="57">
         <v>0.15</v>
       </c>
-      <c r="E49" s="63">
+      <c r="E49" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="62">
+      <c r="A50" s="56">
         <v>48</v>
       </c>
-      <c r="B50" s="62" t="s">
+      <c r="B50" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C50" s="63">
+      <c r="C50" s="57">
         <v>0.2</v>
       </c>
-      <c r="D50" s="63">
+      <c r="D50" s="57">
         <v>0.15</v>
       </c>
-      <c r="E50" s="63">
+      <c r="E50" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="62">
+      <c r="A51" s="56">
         <v>49</v>
       </c>
-      <c r="B51" s="62" t="s">
+      <c r="B51" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C51" s="63">
+      <c r="C51" s="57">
         <v>0.4</v>
       </c>
-      <c r="D51" s="63">
+      <c r="D51" s="57">
         <v>0.15</v>
       </c>
-      <c r="E51" s="63">
+      <c r="E51" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="62">
+      <c r="A52" s="56">
         <v>50</v>
       </c>
-      <c r="B52" s="62" t="s">
+      <c r="B52" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C52" s="63">
+      <c r="C52" s="57">
         <v>0.4</v>
       </c>
-      <c r="D52" s="63">
+      <c r="D52" s="57">
         <v>0.15</v>
       </c>
-      <c r="E52" s="63">
+      <c r="E52" s="57">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="62">
+      <c r="A53" s="56">
         <v>51</v>
       </c>
-      <c r="B53" s="62" t="s">
+      <c r="B53" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C53" s="63">
+      <c r="C53" s="57">
         <v>0.4</v>
       </c>
-      <c r="D53" s="63">
+      <c r="D53" s="57">
         <v>0.15</v>
       </c>
-      <c r="E53" s="63">
+      <c r="E53" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="62">
+      <c r="A54" s="56">
         <v>52</v>
       </c>
-      <c r="B54" s="62" t="s">
+      <c r="B54" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="C54" s="63">
+      <c r="C54" s="57">
         <v>0.4</v>
       </c>
-      <c r="D54" s="63">
+      <c r="D54" s="57">
         <v>0.15</v>
       </c>
-      <c r="E54" s="63">
+      <c r="E54" s="57">
         <v>0.5</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="62">
+      <c r="A55" s="56">
         <v>53</v>
       </c>
-      <c r="B55" s="62" t="s">
+      <c r="B55" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="C55" s="63">
+      <c r="C55" s="57">
         <v>0.4</v>
       </c>
-      <c r="D55" s="63">
+      <c r="D55" s="57">
         <v>0.15</v>
       </c>
-      <c r="E55" s="63">
+      <c r="E55" s="57">
         <v>0.9</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="14" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="64">
+      <c r="A56" s="58">
         <v>54</v>
       </c>
-      <c r="B56" s="64" t="s">
+      <c r="B56" s="58" t="s">
         <v>207</v>
       </c>
-      <c r="C56" s="65">
+      <c r="C56" s="59">
         <v>0.4</v>
       </c>
-      <c r="D56" s="65">
+      <c r="D56" s="59">
         <v>0.15</v>
       </c>
-      <c r="E56" s="65">
+      <c r="E56" s="59">
         <v>0.9</v>
       </c>
     </row>
@@ -8067,22 +9639,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="60" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="59" t="s">
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="65" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="63" t="s">
         <v>204</v>
       </c>
       <c r="I1" s="5"/>
@@ -8102,8 +9674,8 @@
       <c r="F2" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="58"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="64"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" s="14" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9580,9 +11152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AM201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="F191" sqref="F191"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>